<commit_message>
imported exchanges rates.xlsx and suppliers.csv data into warehouse on ssis
</commit_message>
<xml_diff>
--- a/Sql server- SSMS - SSIS/SSMS/table data/exchange_rates.xlsx
+++ b/Sql server- SSMS - SSIS/SSMS/table data/exchange_rates.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7ae6cfe89d2062d/Documents/SQL Server Management Studio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7ae6cfe89d2062d/Documents/DE-practice/Sql server- SSMS - SSIS/SSMS/table data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E63734EA-B30C-4629-9076-FA9A5040A63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB522B8-9F6A-4238-8E46-0FD25C48DB29}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{E63734EA-B30C-4629-9076-FA9A5040A63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD9C00A1-473E-47FF-AD47-B786F1841974}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{E7C8E430-8999-4C97-9459-AFC53CEE48B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rates" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -116,6 +116,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>